<commit_message>
updated to selenium 4.39.0
</commit_message>
<xml_diff>
--- a/target/test-classes/KeywordScenarios/Scenario1.xlsx
+++ b/target/test-classes/KeywordScenarios/Scenario1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
   <si>
     <t>Test Steps</t>
   </si>
@@ -46,25 +46,34 @@
     <t>enter url</t>
   </si>
   <si>
-    <t>http://www.google.com</t>
+    <t>http://mail.google.com</t>
   </si>
   <si>
     <t>enter email address</t>
   </si>
   <si>
-    <t>id=Email</t>
+    <t>id%identifierId</t>
   </si>
   <si>
     <t>sendKeys</t>
   </si>
   <si>
-    <t>virender.kamboj@yahoo.com</t>
+    <t>test.email@gmail.com</t>
+  </si>
+  <si>
+    <t>Click on Next button</t>
+  </si>
+  <si>
+    <t>xpath%//div[@class='VfPpkd-RLmnJb']</t>
+  </si>
+  <si>
+    <t>click</t>
   </si>
   <si>
     <t>enter password</t>
   </si>
   <si>
-    <t>id=Password</t>
+    <t>id%Password</t>
   </si>
   <si>
     <t>Test@123</t>
@@ -73,16 +82,28 @@
     <t>click on Login button</t>
   </si>
   <si>
-    <t>id=LoginButton</t>
-  </si>
-  <si>
-    <t>click</t>
+    <t>id%LoginButton</t>
   </si>
   <si>
     <t>close browser</t>
   </si>
   <si>
     <t>quit</t>
+  </si>
+  <si>
+    <t>clear</t>
+  </si>
+  <si>
+    <t>hover</t>
+  </si>
+  <si>
+    <t>hoverClick</t>
+  </si>
+  <si>
+    <t>selectValue</t>
+  </si>
+  <si>
+    <t>selectIndex</t>
   </si>
 </sst>
 </file>
@@ -113,21 +134,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -135,13 +142,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -163,6 +163,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -173,38 +205,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -219,7 +220,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,13 +249,12 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -242,7 +263,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,109 +284,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,73 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,35 +493,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -521,16 +518,36 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,13 +567,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -574,7 +595,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -592,134 +613,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -730,6 +751,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="10" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1051,16 +1075,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="19" customWidth="1"/>
-    <col min="2" max="2" width="14.6363636363636" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
     <col min="3" max="3" width="13.6363636363636" customWidth="1"/>
     <col min="4" max="4" width="28.4545454545455" customWidth="1"/>
   </cols>
@@ -1129,10 +1153,10 @@
         <v>16</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1143,10 +1167,10 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1154,20 +1178,76 @@
         <v>21</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1"/>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" display="http://www.google.com"/>
-    <hyperlink ref="D4" r:id="rId2" display="virender.kamboj@yahoo.com"/>
-    <hyperlink ref="D5" r:id="rId3" display="Test@123"/>
+    <hyperlink ref="D3" r:id="rId1" display="http://mail.google.com" tooltip="http://mail.google.com"/>
+    <hyperlink ref="D4" r:id="rId2" display="test.email@gmail.com" tooltip="mailto:test.email@gmail.com"/>
+    <hyperlink ref="D6" r:id="rId3" display="Test@123"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>